<commit_message>
updating new version of table2
</commit_message>
<xml_diff>
--- a/src/table2.xlsx
+++ b/src/table2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\קארין\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\קארין\Desktop\Developing-Variety-Of-Methods-For-Identifying-Anomalies-\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,21 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>id</t>
+    <t>Age</t>
   </si>
   <si>
-    <t>age</t>
+    <t>Pulse</t>
   </si>
   <si>
-    <t>pulse</t>
+    <t>SugarBlood</t>
   </si>
   <si>
-    <t>illBefore</t>
-  </si>
-  <si>
-    <t>sugarBlood</t>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -62,12 +59,10 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="5" tint="0.39997558519241921"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="177"/>
-      <scheme val="minor"/>
+      <name val="Lucida Handwriting"/>
+      <family val="4"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,8 +87,12 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB63AC1E-E389-4E60-9806-DF7E4CC6E8D5}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -419,27 +418,23 @@
     <col min="2" max="2" width="20.08203125" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -452,11 +447,8 @@
       <c r="D2" s="1">
         <v>20</v>
       </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -469,11 +461,8 @@
       <c r="D3" s="1">
         <v>50</v>
       </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -481,50 +470,41 @@
         <v>90</v>
       </c>
       <c r="C4" s="1">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D4" s="1">
         <v>41</v>
       </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>130</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>90</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>40</v>
       </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>120</v>
       </c>
-      <c r="C6" s="2">
-        <v>80</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="1">
+        <v>83</v>
+      </c>
+      <c r="D6" s="1">
         <v>50</v>
       </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -532,16 +512,13 @@
         <v>70</v>
       </c>
       <c r="C7" s="1">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D7" s="1">
         <v>21</v>
       </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -549,50 +526,41 @@
         <v>79</v>
       </c>
       <c r="C8" s="1">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D8" s="1">
         <v>22</v>
       </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>118</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>85</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>55</v>
       </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>150</v>
       </c>
-      <c r="C10" s="2">
-        <v>80</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="1">
+        <v>89</v>
+      </c>
+      <c r="D10" s="1">
         <v>57</v>
       </c>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -600,13 +568,80 @@
         <v>78</v>
       </c>
       <c r="C11" s="1">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D11" s="1">
         <v>23</v>
       </c>
-      <c r="E11" s="1">
-        <v>0</v>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>158</v>
+      </c>
+      <c r="C12" s="1">
+        <v>71</v>
+      </c>
+      <c r="D12" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>88</v>
+      </c>
+      <c r="C13" s="1">
+        <v>73</v>
+      </c>
+      <c r="D13" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>89</v>
+      </c>
+      <c r="C14" s="1">
+        <v>77</v>
+      </c>
+      <c r="D14" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>68</v>
+      </c>
+      <c r="C15" s="1">
+        <v>78</v>
+      </c>
+      <c r="D15" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>72</v>
+      </c>
+      <c r="C16" s="1">
+        <v>87</v>
+      </c>
+      <c r="D16" s="1">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>